<commit_message>
Updated on 18th April 2021
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestData.xlsx
+++ b/src/main/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhage\Desktop\swTesting\Project\newPro\LatestFreeCRM\LatestFreeCRM\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6870BE30-D65C-451E-ADC4-6B3DFCE8B8BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF212FAE-5256-463C-A3E3-937F1B9577D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>UserName</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>To Add another Contact to the freeCrm application</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -455,15 +458,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -502,7 +505,9 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -520,7 +525,9 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -534,15 +541,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80D6640-B03D-4753-A75D-7F32A2B2D9FC}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -562,8 +569,10 @@
         <v>12</v>
       </c>
       <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -583,8 +592,10 @@
         <v>18</v>
       </c>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -604,8 +615,10 @@
         <v>18</v>
       </c>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -613,8 +626,10 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -622,8 +637,10 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -631,8 +648,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -640,8 +659,10 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -649,8 +670,10 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -658,6 +681,8 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>